<commit_message>
force undirected, help edits
</commit_message>
<xml_diff>
--- a/pypf/data/bio.prx.xlsx
+++ b/pypf/data/bio.prx.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schva\Prog\MATLAB\network\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schva\Prog\py_proj\pypf\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B4554644-A9A6-4A71-BB00-5E0F46C0292B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C964130-6154-4437-B94D-C689715264F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17205" yWindow="450" windowWidth="17040" windowHeight="14190" xr2:uid="{FF22AAE5-3D6D-478D-AD3E-8244737B6671}"/>
+    <workbookView xWindow="-17925" yWindow="1290" windowWidth="12045" windowHeight="13665" xr2:uid="{FF22AAE5-3D6D-478D-AD3E-8244737B6671}"/>
   </bookViews>
   <sheets>
     <sheet name="natbioDistances" sheetId="1" r:id="rId1"/>
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="26">
-  <si>
-    <t>Row</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="25">
   <si>
     <t>living thing</t>
   </si>
@@ -581,8 +578,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -960,93 +960,96 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2781BEB5-9577-49D1-8624-F2FDBC508EAC}">
   <dimension ref="A1:Z26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AB10" sqref="AB10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="26" width="3.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:26" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1126,7 +1129,7 @@
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>32</v>
@@ -1206,7 +1209,7 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>40</v>
@@ -1286,7 +1289,7 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>32</v>
@@ -1366,7 +1369,7 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>73</v>
@@ -1446,7 +1449,7 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>37</v>
@@ -1526,7 +1529,7 @@
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>33</v>
@@ -1606,7 +1609,7 @@
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>27</v>
@@ -1686,7 +1689,7 @@
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>65</v>
@@ -1766,7 +1769,7 @@
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>36</v>
@@ -1846,7 +1849,7 @@
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>27</v>
@@ -1926,7 +1929,7 @@
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>33</v>
@@ -2006,7 +2009,7 @@
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>61</v>
@@ -2086,7 +2089,7 @@
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>74</v>
@@ -2166,7 +2169,7 @@
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>40</v>
@@ -2246,7 +2249,7 @@
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>33</v>
@@ -2326,7 +2329,7 @@
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>50</v>
@@ -2406,7 +2409,7 @@
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>28</v>
@@ -2486,7 +2489,7 @@
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>44</v>
@@ -2566,7 +2569,7 @@
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
         <v>36</v>
@@ -2646,7 +2649,7 @@
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
         <v>34</v>
@@ -2726,7 +2729,7 @@
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
         <v>34</v>
@@ -2806,7 +2809,7 @@
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
         <v>60</v>
@@ -2886,7 +2889,7 @@
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
         <v>59</v>
@@ -2966,7 +2969,7 @@
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26">
         <v>71</v>

</xml_diff>